<commit_message>
rekap formulir Fin done,report portal fin html done
</commit_message>
<xml_diff>
--- a/uploads/finance/TemplateRekapFormulir.xlsx
+++ b/uploads/finance/TemplateRekapFormulir.xlsx
@@ -424,7 +424,7 @@
   <dimension ref="B1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,12 +475,8 @@
       <c r="I5" s="6"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="7">
-        <v>1</v>
-      </c>
-      <c r="C6" s="7">
-        <v>190000</v>
-      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>

</xml_diff>

<commit_message>
Update Kwitansi dan Report Formulir Offline & Online
</commit_message>
<xml_diff>
--- a/uploads/finance/TemplateRekapFormulir.xlsx
+++ b/uploads/finance/TemplateRekapFormulir.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\puis\uploads\finance\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0D48D4-D344-45CA-ACA2-BAE0B2061DFD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21585" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Form Pendaftaran TA 2019/2020</t>
   </si>
@@ -51,12 +52,18 @@
   </si>
   <si>
     <t>Belum terjual/ belum ada pembayaran untuk nomer formulir ini</t>
+  </si>
+  <si>
+    <t>Kwitansi</t>
+  </si>
+  <si>
+    <t>Tipe Formulir</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -88,7 +95,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -111,15 +118,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -133,7 +131,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -141,6 +138,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,11 +420,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,26 +433,27 @@
     <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
@@ -468,20 +469,27 @@
       <c r="F5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="5" t="s">
+      <c r="G5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="6"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="H6" s="8"/>
-      <c r="I6" t="s">
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="7"/>
+      <c r="J6" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>